<commit_message>
Added Shortlist Sheet to Variable_List Excel'
</commit_message>
<xml_diff>
--- a/Meeting Minutes.xlsx
+++ b/Meeting Minutes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Day</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">Do read up on Public Kernels to get a balanced picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picked Significant Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to impute/transform/engineer features by this Friday</t>
   </si>
 </sst>
 </file>
@@ -71,6 +80,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -143,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -158,6 +168,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -237,16 +251,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
@@ -319,11 +333,36 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>43040</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>